<commit_message>
Added Percent Interpretation to JSON
</commit_message>
<xml_diff>
--- a/src/configs/Degen_Doods.xlsx
+++ b/src/configs/Degen_Doods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joser\OneDrive\Documents\GitHub\pfpgen\src\collections\Degen Doodz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f30736e284a438bb/Documents/GitHub/pfpgen/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E106BAFF-0171-4D50-BCEC-CAD845A7F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E106BAFF-0171-4D50-BCEC-CAD845A7F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52C865AA-6BB6-4F07-9231-5C94579BAAE4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E70FE35A-380B-CA41-BF02-0C6C7926FEE3}"/>
+    <workbookView xWindow="3375" yWindow="645" windowWidth="27315" windowHeight="14235" xr2:uid="{E70FE35A-380B-CA41-BF02-0C6C7926FEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -618,35 +620,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -681,8 +659,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1001,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9A3DD8-4154-044E-9F1E-75A75344028B}">
   <dimension ref="A1:AT187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4:AA16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1047,16 +1049,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:46" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="14"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
@@ -1076,41 +1078,41 @@
       <c r="AP1" s="2"/>
     </row>
     <row r="2" spans="2:46" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="51" t="s">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="51" t="s">
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="37" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="39"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="46"/>
       <c r="AF2" s="32"/>
       <c r="AG2" s="32"/>
       <c r="AH2" s="32"/>
@@ -3337,11 +3339,11 @@
       <c r="AT32" s="2"/>
     </row>
     <row r="33" spans="1:43" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="45">
+      <c r="B33" s="37">
         <v>5555</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
       <c r="AL33" s="2"/>
@@ -3351,9 +3353,9 @@
       <c r="AP33" s="2"/>
     </row>
     <row r="34" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="48"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
@@ -4944,9 +4946,9 @@
     </row>
     <row r="71" spans="1:43" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="B71" s="51"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -4989,41 +4991,41 @@
     </row>
     <row r="72" spans="1:43" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
-      <c r="B72" s="33"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
-      <c r="K72" s="31"/>
-      <c r="L72" s="31"/>
-      <c r="M72" s="31"/>
-      <c r="N72" s="31"/>
-      <c r="O72" s="31"/>
-      <c r="P72" s="31"/>
-      <c r="Q72" s="31"/>
-      <c r="R72" s="31"/>
-      <c r="S72" s="31"/>
-      <c r="T72" s="31"/>
-      <c r="U72" s="31"/>
-      <c r="V72" s="31"/>
-      <c r="W72" s="31"/>
-      <c r="X72" s="31"/>
-      <c r="Y72" s="31"/>
-      <c r="Z72" s="31"/>
-      <c r="AA72" s="31"/>
-      <c r="AB72" s="31"/>
-      <c r="AC72" s="31"/>
-      <c r="AD72" s="31"/>
-      <c r="AE72" s="31"/>
-      <c r="AF72" s="31"/>
-      <c r="AG72" s="31"/>
-      <c r="AH72" s="31"/>
-      <c r="AI72" s="31"/>
-      <c r="AJ72" s="31"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="48"/>
+      <c r="I72" s="48"/>
+      <c r="J72" s="48"/>
+      <c r="K72" s="48"/>
+      <c r="L72" s="48"/>
+      <c r="M72" s="48"/>
+      <c r="N72" s="48"/>
+      <c r="O72" s="48"/>
+      <c r="P72" s="48"/>
+      <c r="Q72" s="48"/>
+      <c r="R72" s="48"/>
+      <c r="S72" s="48"/>
+      <c r="T72" s="48"/>
+      <c r="U72" s="48"/>
+      <c r="V72" s="48"/>
+      <c r="W72" s="48"/>
+      <c r="X72" s="48"/>
+      <c r="Y72" s="48"/>
+      <c r="Z72" s="48"/>
+      <c r="AA72" s="48"/>
+      <c r="AB72" s="48"/>
+      <c r="AC72" s="48"/>
+      <c r="AD72" s="48"/>
+      <c r="AE72" s="48"/>
+      <c r="AF72" s="48"/>
+      <c r="AG72" s="48"/>
+      <c r="AH72" s="48"/>
+      <c r="AI72" s="48"/>
+      <c r="AJ72" s="48"/>
       <c r="AK72" s="2"/>
       <c r="AL72" s="2"/>
       <c r="AM72" s="2"/>
@@ -5214,91 +5216,91 @@
     </row>
     <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="36"/>
-      <c r="K77" s="36"/>
-      <c r="L77" s="36"/>
-      <c r="M77" s="36"/>
-      <c r="N77" s="36"/>
-      <c r="O77" s="36"/>
-      <c r="P77" s="36"/>
-      <c r="Q77" s="36"/>
-      <c r="R77" s="36"/>
-      <c r="S77" s="36"/>
-      <c r="T77" s="36"/>
-      <c r="U77" s="36"/>
-      <c r="V77" s="36"/>
-      <c r="W77" s="36"/>
-      <c r="X77" s="36"/>
-      <c r="Y77" s="36"/>
-      <c r="Z77" s="36"/>
-      <c r="AA77" s="36"/>
-      <c r="AB77" s="36"/>
-      <c r="AC77" s="36"/>
-      <c r="AD77" s="36"/>
-      <c r="AE77" s="36"/>
-      <c r="AF77" s="36"/>
-      <c r="AG77" s="36"/>
-      <c r="AH77" s="36"/>
-      <c r="AI77" s="36"/>
-      <c r="AJ77" s="36"/>
-      <c r="AK77" s="36"/>
-      <c r="AL77" s="36"/>
-      <c r="AM77" s="36"/>
-      <c r="AN77" s="36"/>
-      <c r="AO77" s="36"/>
+      <c r="B77" s="51"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="47"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="47"/>
+      <c r="J77" s="47"/>
+      <c r="K77" s="47"/>
+      <c r="L77" s="47"/>
+      <c r="M77" s="47"/>
+      <c r="N77" s="47"/>
+      <c r="O77" s="47"/>
+      <c r="P77" s="47"/>
+      <c r="Q77" s="47"/>
+      <c r="R77" s="47"/>
+      <c r="S77" s="47"/>
+      <c r="T77" s="47"/>
+      <c r="U77" s="47"/>
+      <c r="V77" s="47"/>
+      <c r="W77" s="47"/>
+      <c r="X77" s="47"/>
+      <c r="Y77" s="47"/>
+      <c r="Z77" s="47"/>
+      <c r="AA77" s="47"/>
+      <c r="AB77" s="47"/>
+      <c r="AC77" s="47"/>
+      <c r="AD77" s="47"/>
+      <c r="AE77" s="47"/>
+      <c r="AF77" s="47"/>
+      <c r="AG77" s="47"/>
+      <c r="AH77" s="47"/>
+      <c r="AI77" s="47"/>
+      <c r="AJ77" s="47"/>
+      <c r="AK77" s="47"/>
+      <c r="AL77" s="47"/>
+      <c r="AM77" s="47"/>
+      <c r="AN77" s="47"/>
+      <c r="AO77" s="47"/>
       <c r="AP77" s="2"/>
       <c r="AQ77" s="2"/>
     </row>
     <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="36"/>
-      <c r="I78" s="36"/>
-      <c r="J78" s="36"/>
-      <c r="K78" s="36"/>
-      <c r="L78" s="36"/>
-      <c r="M78" s="36"/>
-      <c r="N78" s="36"/>
-      <c r="O78" s="36"/>
-      <c r="P78" s="36"/>
-      <c r="Q78" s="36"/>
-      <c r="R78" s="36"/>
-      <c r="S78" s="36"/>
-      <c r="T78" s="36"/>
-      <c r="U78" s="36"/>
-      <c r="V78" s="36"/>
-      <c r="W78" s="36"/>
-      <c r="X78" s="36"/>
-      <c r="Y78" s="36"/>
-      <c r="Z78" s="36"/>
-      <c r="AA78" s="36"/>
-      <c r="AB78" s="36"/>
-      <c r="AC78" s="36"/>
-      <c r="AD78" s="36"/>
-      <c r="AE78" s="36"/>
-      <c r="AF78" s="36"/>
-      <c r="AG78" s="36"/>
-      <c r="AH78" s="36"/>
-      <c r="AI78" s="36"/>
-      <c r="AJ78" s="36"/>
-      <c r="AK78" s="36"/>
-      <c r="AL78" s="36"/>
-      <c r="AM78" s="36"/>
-      <c r="AN78" s="36"/>
-      <c r="AO78" s="36"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="47"/>
+      <c r="I78" s="47"/>
+      <c r="J78" s="47"/>
+      <c r="K78" s="47"/>
+      <c r="L78" s="47"/>
+      <c r="M78" s="47"/>
+      <c r="N78" s="47"/>
+      <c r="O78" s="47"/>
+      <c r="P78" s="47"/>
+      <c r="Q78" s="47"/>
+      <c r="R78" s="47"/>
+      <c r="S78" s="47"/>
+      <c r="T78" s="47"/>
+      <c r="U78" s="47"/>
+      <c r="V78" s="47"/>
+      <c r="W78" s="47"/>
+      <c r="X78" s="47"/>
+      <c r="Y78" s="47"/>
+      <c r="Z78" s="47"/>
+      <c r="AA78" s="47"/>
+      <c r="AB78" s="47"/>
+      <c r="AC78" s="47"/>
+      <c r="AD78" s="47"/>
+      <c r="AE78" s="47"/>
+      <c r="AF78" s="47"/>
+      <c r="AG78" s="47"/>
+      <c r="AH78" s="47"/>
+      <c r="AI78" s="47"/>
+      <c r="AJ78" s="47"/>
+      <c r="AK78" s="47"/>
+      <c r="AL78" s="47"/>
+      <c r="AM78" s="47"/>
+      <c r="AN78" s="47"/>
+      <c r="AO78" s="47"/>
       <c r="AP78" s="2"/>
       <c r="AQ78" s="2"/>
     </row>
@@ -5486,10 +5488,10 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
+      <c r="D83" s="52"/>
+      <c r="E83" s="52"/>
+      <c r="F83" s="52"/>
+      <c r="G83" s="52"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
@@ -6249,41 +6251,41 @@
     </row>
     <row r="100" spans="1:43" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="31"/>
-      <c r="F100" s="31"/>
-      <c r="G100" s="35"/>
-      <c r="H100" s="35"/>
-      <c r="I100" s="35"/>
-      <c r="J100" s="35"/>
-      <c r="K100" s="35"/>
-      <c r="L100" s="31"/>
-      <c r="M100" s="31"/>
-      <c r="N100" s="31"/>
-      <c r="O100" s="31"/>
-      <c r="P100" s="31"/>
-      <c r="Q100" s="31"/>
-      <c r="R100" s="31"/>
-      <c r="S100" s="31"/>
-      <c r="T100" s="31"/>
-      <c r="U100" s="31"/>
-      <c r="V100" s="31"/>
-      <c r="W100" s="31"/>
-      <c r="X100" s="31"/>
-      <c r="Y100" s="31"/>
-      <c r="Z100" s="31"/>
-      <c r="AA100" s="31"/>
-      <c r="AB100" s="31"/>
-      <c r="AC100" s="31"/>
-      <c r="AD100" s="31"/>
-      <c r="AE100" s="31"/>
-      <c r="AF100" s="31"/>
-      <c r="AG100" s="31"/>
-      <c r="AH100" s="31"/>
-      <c r="AI100" s="31"/>
-      <c r="AJ100" s="31"/>
+      <c r="B100" s="48"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="48"/>
+      <c r="E100" s="48"/>
+      <c r="F100" s="48"/>
+      <c r="G100" s="50"/>
+      <c r="H100" s="50"/>
+      <c r="I100" s="50"/>
+      <c r="J100" s="50"/>
+      <c r="K100" s="50"/>
+      <c r="L100" s="48"/>
+      <c r="M100" s="48"/>
+      <c r="N100" s="48"/>
+      <c r="O100" s="48"/>
+      <c r="P100" s="48"/>
+      <c r="Q100" s="48"/>
+      <c r="R100" s="48"/>
+      <c r="S100" s="48"/>
+      <c r="T100" s="48"/>
+      <c r="U100" s="48"/>
+      <c r="V100" s="48"/>
+      <c r="W100" s="48"/>
+      <c r="X100" s="48"/>
+      <c r="Y100" s="48"/>
+      <c r="Z100" s="48"/>
+      <c r="AA100" s="48"/>
+      <c r="AB100" s="48"/>
+      <c r="AC100" s="48"/>
+      <c r="AD100" s="48"/>
+      <c r="AE100" s="48"/>
+      <c r="AF100" s="48"/>
+      <c r="AG100" s="48"/>
+      <c r="AH100" s="48"/>
+      <c r="AI100" s="48"/>
+      <c r="AJ100" s="48"/>
       <c r="AK100" s="2"/>
       <c r="AL100" s="2"/>
       <c r="AM100" s="2"/>
@@ -9873,27 +9875,16 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="B33:D34"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="AK77:AO78"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AF38:AJ38"/>
-    <mergeCell ref="AK38:AO38"/>
-    <mergeCell ref="V72:Z72"/>
-    <mergeCell ref="AA72:AE72"/>
-    <mergeCell ref="AF72:AJ72"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="V100:Z100"/>
+    <mergeCell ref="Q72:U72"/>
+    <mergeCell ref="AA100:AE100"/>
+    <mergeCell ref="AF100:AJ100"/>
+    <mergeCell ref="V38:Z38"/>
+    <mergeCell ref="AA38:AE38"/>
+    <mergeCell ref="Q38:U38"/>
+    <mergeCell ref="V77:Z78"/>
+    <mergeCell ref="AA77:AE78"/>
+    <mergeCell ref="AF77:AJ78"/>
+    <mergeCell ref="Q77:U78"/>
     <mergeCell ref="B71:D72"/>
     <mergeCell ref="D83:G83"/>
     <mergeCell ref="B38:F38"/>
@@ -9905,16 +9896,27 @@
     <mergeCell ref="G77:K78"/>
     <mergeCell ref="L77:P78"/>
     <mergeCell ref="L72:P72"/>
-    <mergeCell ref="Q72:U72"/>
-    <mergeCell ref="AA100:AE100"/>
-    <mergeCell ref="AF100:AJ100"/>
-    <mergeCell ref="V38:Z38"/>
-    <mergeCell ref="AA38:AE38"/>
-    <mergeCell ref="Q38:U38"/>
-    <mergeCell ref="V77:Z78"/>
-    <mergeCell ref="AA77:AE78"/>
-    <mergeCell ref="AF77:AJ78"/>
-    <mergeCell ref="Q77:U78"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="V100:Z100"/>
+    <mergeCell ref="AK77:AO78"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AF38:AJ38"/>
+    <mergeCell ref="AK38:AO38"/>
+    <mergeCell ref="V72:Z72"/>
+    <mergeCell ref="AA72:AE72"/>
+    <mergeCell ref="AF72:AJ72"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="B33:D34"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>